<commit_message>
the form now has 3 screens, but it contain bugs
</commit_message>
<xml_diff>
--- a/data/template_orcamento.xlsx
+++ b/data/template_orcamento.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d6f4c746525ba205/Documentos/Projetos pessoais/Projeto_Buffet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\davil\Projects\BuffetAutomatization\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{749B7E60-4BE6-46AA-92F5-8850F3AD870A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA0EA40-06B8-4E92-8FE1-2136C3BCDCD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{559E694E-777D-4259-8B61-B07215B4A515}"/>
   </bookViews>
@@ -95,12 +95,6 @@
     <t>Valor  Total:</t>
   </si>
   <si>
-    <t>1_opcao</t>
-  </si>
-  <si>
-    <t>2_opcao</t>
-  </si>
-  <si>
     <t>Observações:</t>
   </si>
   <si>
@@ -165,6 +159,12 @@
   </si>
   <si>
     <t>{type_recepcao}</t>
+  </si>
+  <si>
+    <t>{1_opcao}</t>
+  </si>
+  <si>
+    <t>{2_opcao}</t>
   </si>
 </sst>
 </file>
@@ -274,18 +274,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -293,20 +313,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5BF5916-F660-4136-B6CD-6E3458A9E384}">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:H9"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,326 +658,323 @@
     <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="24" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:15" ht="24" x14ac:dyDescent="0.5">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-    </row>
-    <row r="2" spans="1:12" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+    </row>
+    <row r="2" spans="1:15" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11" t="s">
+    <row r="5" spans="1:15" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="11" t="s">
+    <row r="6" spans="1:15" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="11" t="s">
+    <row r="8" spans="1:15" ht="21.6" x14ac:dyDescent="0.45">
+      <c r="A8" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="11" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="21.6" x14ac:dyDescent="0.45">
+      <c r="A11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="13" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="1:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A19" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="11"/>
+    </row>
+    <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
+      <c r="A25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="21.6" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="21.6" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="L14" s="13"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
-      <c r="A20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="4" t="s">
+    <row r="30" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
+      <c r="A31" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="A32" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="34" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
+      <c r="A34" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="6"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
+      <c r="A37" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
+      <c r="A40" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+    </row>
+    <row r="41" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="A41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="4" t="s">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A45" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
-      <c r="A25" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
-      <c r="A27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
-      <c r="A29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
-      <c r="A31" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-    </row>
-    <row r="32" spans="1:8" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
+      <c r="B45" s="9"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A39" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
+      <c r="C46" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="A39:H39"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A25:H25"/>
+  <mergeCells count="3">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A8:H8"/>
     <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A16:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add Mao de Obra, Opções de Prato Principal no formulário
</commit_message>
<xml_diff>
--- a/data/template_orcamento.xlsx
+++ b/data/template_orcamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\davil\Projects\BuffetAutomatization\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA0EA40-06B8-4E92-8FE1-2136C3BCDCD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4413B8F-289A-4F03-97CD-8D7A45D14789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{559E694E-777D-4259-8B61-B07215B4A515}"/>
   </bookViews>
@@ -647,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5BF5916-F660-4136-B6CD-6E3458A9E384}">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -858,12 +858,6 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A28" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -871,26 +865,27 @@
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
+      <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
-      <c r="A31" s="6" t="s">
+    <row r="32" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
+      <c r="A32" s="6" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A32" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -900,31 +895,35 @@
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
     </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="34" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
-      <c r="A34" s="6" t="s">
+      <c r="B34" s="6"/>
+    </row>
+    <row r="35" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
+      <c r="A35" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="6"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
-      <c r="A37" s="6" t="s">
+    <row r="38" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
+      <c r="A38" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
-      <c r="A40" s="6" t="s">
-        <v>16</v>
-      </c>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
@@ -932,9 +931,9 @@
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
     </row>
-    <row r="41" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="A41" s="1" t="s">
-        <v>17</v>
+    <row r="41" spans="1:8" ht="21.6" x14ac:dyDescent="0.45">
+      <c r="A41" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="9"/>
@@ -943,32 +942,35 @@
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="B42" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:8" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A45" s="8" t="s">
+    <row r="46" spans="1:8" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A46" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="9"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="s">
+      <c r="B46" s="9"/>
+      <c r="C46" s="5"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>